<commit_message>
added code to run on docker
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
   <si>
     <t>testname</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>79.0.3945.117</t>
+  </si>
+  <si>
+    <t>88.0.4324.96</t>
+  </si>
+  <si>
+    <t>69.0</t>
   </si>
 </sst>
 </file>
@@ -459,7 +471,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,23 +559,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E6"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.26953125" customWidth="1"/>
     <col min="2" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="6" max="6" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,19 +587,22 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -596,20 +612,23 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -619,20 +638,23 @@
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,20 +664,23 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -665,20 +690,23 @@
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -688,20 +716,23 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -711,8 +742,8 @@
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
@@ -720,7 +751,62 @@
       <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ELK Utils and Updated docker compose file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -525,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>23</v>
@@ -633,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -659,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -711,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Optimised Data Provider Utils code with RemoveIf
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -122,8 +122,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,10 +256,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,7 +290,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,23 +465,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:5" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:5" ht="28.8">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -517,7 +515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -534,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:5" ht="28.8">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -558,25 +556,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6328125" customWidth="1"/>
-    <col min="6" max="6" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:8" ht="28.8">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -628,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:8" ht="28.8">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:8" ht="28.8">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -680,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:8" ht="28.8">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,7 +704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -732,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:8" ht="28.8">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -758,12 +756,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:8" ht="28.8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -784,7 +782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:8" ht="34.049999999999997" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>